<commit_message>
MicroSoft™ Engineer™ Certified™ Document™ added™
</commit_message>
<xml_diff>
--- a/reports/images/ProjectPlan.xlsx
+++ b/reports/images/ProjectPlan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\GitHub\CS4470Y\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\GitHub\CS4470Y\reports\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="71">
   <si>
     <t>Project Planner</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Feature 9</t>
   </si>
   <si>
-    <t>Feature 10</t>
-  </si>
-  <si>
     <t>FR 1</t>
   </si>
   <si>
@@ -191,84 +188,9 @@
     <t>FR 3</t>
   </si>
   <si>
-    <t>QR 1</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>Extract commits from a .git directory</t>
-  </si>
-  <si>
-    <t>Analyze and record classes/methods effected by each commit</t>
-  </si>
-  <si>
-    <t>Process and record the amount of code changed with each commit</t>
-  </si>
-  <si>
-    <t>Record results of the test suite each time it is run</t>
-  </si>
-  <si>
-    <t>During test phase inject previous risk analysis</t>
-  </si>
-  <si>
-    <t>Record issues filed for the code base</t>
-  </si>
-  <si>
-    <t>Connect issues to their resolution and make an inference from the association</t>
-  </si>
-  <si>
-    <t>Allow parsing from diverse options (User newsgroups, technical reports, etc)</t>
-  </si>
-  <si>
-    <t>Standardize and combine Git data into a central data model</t>
-  </si>
-  <si>
-    <t>Standardize and combine test data into a central data model</t>
-  </si>
-  <si>
-    <t>Standardize and combine issue data into a central data model</t>
-  </si>
-  <si>
-    <t>In the data model figure out risky parts of the code and mark them</t>
-  </si>
-  <si>
-    <t>Identify issue keywords that are higher risk than others</t>
-  </si>
-  <si>
-    <t>Identify impact when a test is changed (how much coverage it offers)</t>
-  </si>
-  <si>
-    <t>Create a PDF report for stakeholders to see progress in codebase</t>
-  </si>
-  <si>
-    <t>Create a Web view for exploring the risk of the codebase</t>
-  </si>
-  <si>
-    <t>Create Github, IFTTT and Slack integrations for viewing framework data model</t>
-  </si>
-  <si>
-    <t>Create test integration so developer can see risk rating when conducting tests</t>
-  </si>
-  <si>
-    <t>Develop command line interface to the framework</t>
-  </si>
-  <si>
-    <t>Research deployment frameworks and integrate risk analysis into pipe line</t>
-  </si>
-  <si>
-    <t>Develop VIM plugin for viewing risk rating of each method/class</t>
-  </si>
-  <si>
-    <t>Develop IDEA plugin for viewing risk rating of each method/class</t>
-  </si>
-  <si>
-    <t>Make the framework easily deployable into a microservice</t>
-  </si>
-  <si>
-    <t>Reduce dependencies and deliver a minimally intrusive product</t>
-  </si>
-  <si>
     <t>Frameworks to Support Continuous Delivery</t>
   </si>
   <si>
@@ -315,6 +237,90 @@
   </si>
   <si>
     <t>Initial meeting with professor for requirements</t>
+  </si>
+  <si>
+    <t>Pass code through cdif2rsf to generate rsf</t>
+  </si>
+  <si>
+    <t>Clean up incorrect entity and relationships</t>
+  </si>
+  <si>
+    <t>Store in accessible data storage for next step to use</t>
+  </si>
+  <si>
+    <t>Compare each token to codebase to find valid functions</t>
+  </si>
+  <si>
+    <t>Expand initial token set by a factor of 3</t>
+  </si>
+  <si>
+    <t>Use NLP to determine question context</t>
+  </si>
+  <si>
+    <t>Run LSI on each token and generate search space for each</t>
+  </si>
+  <si>
+    <t>Expand the search space for each result in FR 1</t>
+  </si>
+  <si>
+    <t>Find similarities between the initial token expansion and the final set of tokens</t>
+  </si>
+  <si>
+    <t>FR 4</t>
+  </si>
+  <si>
+    <t>Apply ranking equation from research paper to come up with final outcome</t>
+  </si>
+  <si>
+    <t>Scan user’s Github repos using Github’s API</t>
+  </si>
+  <si>
+    <t>Allow the user to select ones they wish to run processing on</t>
+  </si>
+  <si>
+    <t>Remember which ones the user selected by storing on backend</t>
+  </si>
+  <si>
+    <t>Monitor output from backend endpoints showing new results for user’s repos</t>
+  </si>
+  <si>
+    <t>When a new bug report is created, and the processing finishes, show the output of that processing on a separate page</t>
+  </si>
+  <si>
+    <t>Allow the user to rerun processing on a specific bug report by sending a request to backend</t>
+  </si>
+  <si>
+    <t>On first usage redirect user to Github’s App authentication page</t>
+  </si>
+  <si>
+    <t>Ask backend to associate bug reports and repositories with this user</t>
+  </si>
+  <si>
+    <t>Redirect user to main UI</t>
+  </si>
+  <si>
+    <t>Allow registration using Github Auth</t>
+  </si>
+  <si>
+    <t>Allow retrieval of processing results for each bug report</t>
+  </si>
+  <si>
+    <t>Automate RSF generation when a new repository is linked</t>
+  </si>
+  <si>
+    <t>Automate keyword generation when a new repository is linked</t>
+  </si>
+  <si>
+    <t>Continuously improve and modify RSF and keywords as code/bugs change</t>
+  </si>
+  <si>
+    <t>Monitor marked repositories for each registered user and trigger when new issue is filed</t>
+  </si>
+  <si>
+    <t>Run through automated ranking algorithm</t>
+  </si>
+  <si>
+    <t>Store result for later retrieval</t>
   </si>
 </sst>
 </file>
@@ -324,7 +330,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -442,13 +448,6 @@
       <i/>
       <sz val="14"/>
       <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -673,7 +672,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,9 +742,6 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -856,9 +852,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -882,7 +875,7 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="122">
     <dxf>
       <fill>
         <patternFill>
@@ -1338,6 +1331,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1349,19 +1370,75 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
         </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1477,14 +1554,1060 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9966FF"/>
       <color rgb="FF00FF99"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF0099FF"/>
-      <color rgb="FF9966FF"/>
       <color rgb="FF9933FF"/>
     </mruColors>
   </colors>
@@ -1730,10 +2853,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:HH35"/>
+  <dimension ref="B1:HH39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1742,7 +2865,7 @@
     <col min="2" max="2" width="13" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="70.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12" style="30" customWidth="1"/>
     <col min="6" max="6" width="11.625" style="16" customWidth="1"/>
     <col min="7" max="7" width="11.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.625" style="16" customWidth="1"/>
@@ -1753,85 +2876,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:216" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="2:216" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>57</v>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:216" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
+      <c r="B3" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
       <c r="J3"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="54"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="52" t="s">
+      <c r="R3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="53"/>
       <c r="V3" s="10"/>
-      <c r="W3" s="56" t="s">
+      <c r="W3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="58"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="57"/>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="41" t="s">
+      <c r="AB3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="34"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="33"/>
       <c r="AG3" s="12"/>
-      <c r="AH3" s="41" t="s">
+      <c r="AH3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" s="42"/>
-      <c r="AJ3" s="42"/>
-      <c r="AK3" s="42"/>
-      <c r="AL3" s="42"/>
-      <c r="AO3" s="34"/>
-      <c r="AP3" s="34"/>
-      <c r="AQ3" s="34"/>
+      <c r="AI3" s="41"/>
+      <c r="AJ3" s="41"/>
+      <c r="AK3" s="41"/>
+      <c r="AL3" s="41"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="33"/>
+      <c r="AQ3" s="33"/>
       <c r="AR3"/>
       <c r="AS3"/>
       <c r="AT3"/>
@@ -1841,31 +2964,31 @@
       <c r="AX3"/>
     </row>
     <row r="4" spans="2:216" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="46" t="s">
+      <c r="D4" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="50" t="s">
+      <c r="J4" s="49" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="13" t="s">
@@ -1931,15 +3054,15 @@
       <c r="BQ4" s="5"/>
     </row>
     <row r="5" spans="2:216" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="51"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="50"/>
       <c r="K5" s="14">
         <v>42991</v>
       </c>
@@ -2560,17 +3683,17 @@
       </c>
     </row>
     <row r="6" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
-        <v>59</v>
+      <c r="B6" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="F6" s="19">
         <v>42991</v>
@@ -2587,20 +3710,20 @@
       <c r="J6" s="22">
         <v>1</v>
       </c>
-      <c r="K6" s="33"/>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
-        <v>59</v>
+      <c r="B7" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>60</v>
+        <v>42</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="F7" s="19">
         <v>43013</v>
@@ -2619,17 +3742,17 @@
       </c>
     </row>
     <row r="8" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
-        <v>59</v>
+      <c r="B8" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>60</v>
+        <v>36</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="F8" s="19">
         <v>43027</v>
@@ -2648,17 +3771,17 @@
       </c>
     </row>
     <row r="9" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
-        <v>59</v>
+      <c r="B9" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="F9" s="19">
         <v>43028</v>
@@ -2677,17 +3800,17 @@
       </c>
     </row>
     <row r="10" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
-        <v>59</v>
+      <c r="B10" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>60</v>
+        <v>37</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="F10" s="19">
         <v>43028</v>
@@ -2706,17 +3829,17 @@
       </c>
     </row>
     <row r="11" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
-        <v>59</v>
+      <c r="B11" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>64</v>
+        <v>40</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="F11" s="19">
         <v>43028</v>
@@ -2735,113 +3858,101 @@
       </c>
     </row>
     <row r="12" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F12" s="19">
-        <v>43033</v>
+        <v>43151</v>
       </c>
       <c r="G12" s="20">
         <v>2</v>
       </c>
-      <c r="H12" s="61">
-        <v>43047</v>
-      </c>
-      <c r="I12" s="20">
-        <v>2</v>
-      </c>
+      <c r="H12"/>
+      <c r="I12"/>
       <c r="J12" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>64</v>
+        <v>44</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F13" s="19">
         <f>G12+F12</f>
-        <v>43035</v>
+        <v>43153</v>
       </c>
       <c r="G13" s="20">
-        <v>5</v>
-      </c>
-      <c r="H13" s="19">
-        <v>43053</v>
-      </c>
-      <c r="I13" s="20">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13"/>
       <c r="J13" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>61</v>
+        <v>45</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F14" s="19">
-        <f t="shared" ref="F14:F35" si="0">G13+F13</f>
-        <v>43040</v>
+        <f t="shared" ref="F14:F39" si="0">G13+F13</f>
+        <v>43155</v>
       </c>
       <c r="G14" s="20">
-        <v>4</v>
-      </c>
-      <c r="H14" s="19">
-        <v>43067</v>
-      </c>
-      <c r="I14" s="20">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14"/>
       <c r="J14" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>64</v>
+        <v>46</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F15" s="19">
         <f t="shared" si="0"/>
-        <v>43044</v>
+        <v>43156</v>
       </c>
       <c r="G15" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="20"/>
@@ -2850,24 +3961,24 @@
       </c>
     </row>
     <row r="16" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F16" s="19">
         <f t="shared" si="0"/>
-        <v>43046</v>
+        <v>43157</v>
       </c>
       <c r="G16" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="20"/>
@@ -2876,24 +3987,24 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
-        <v>16</v>
+      <c r="B17" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F17" s="19">
         <f t="shared" si="0"/>
-        <v>43049</v>
+        <v>43159</v>
       </c>
       <c r="G17" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20"/>
@@ -2902,24 +4013,24 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>64</v>
+        <v>49</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F18" s="19">
         <f t="shared" si="0"/>
-        <v>43052</v>
+        <v>43160</v>
       </c>
       <c r="G18" s="20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="20"/>
@@ -2928,24 +4039,24 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
-        <v>17</v>
+      <c r="B19" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="37" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F19" s="19">
         <f t="shared" si="0"/>
-        <v>43058</v>
+        <v>43161</v>
       </c>
       <c r="G19" s="20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="20"/>
@@ -2954,24 +4065,24 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
-        <v>18</v>
+      <c r="B20" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F20" s="19">
         <f t="shared" si="0"/>
-        <v>43063</v>
+        <v>43162</v>
       </c>
       <c r="G20" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="20"/>
@@ -2980,24 +4091,24 @@
       </c>
     </row>
     <row r="21" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
-        <v>18</v>
+      <c r="B21" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D21" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="35" t="s">
         <v>38</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>64</v>
       </c>
       <c r="F21" s="19">
         <f t="shared" si="0"/>
-        <v>43067</v>
+        <v>43164</v>
       </c>
       <c r="G21" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="20"/>
@@ -3006,24 +4117,24 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="25" t="s">
-        <v>18</v>
+      <c r="B22" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>61</v>
+        <v>54</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="F22" s="19">
         <f t="shared" si="0"/>
-        <v>43070</v>
+        <v>43166</v>
       </c>
       <c r="G22" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="20"/>
@@ -3032,23 +4143,24 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
-        <v>19</v>
+      <c r="B23" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F23" s="19">
-        <v>43103</v>
+        <f t="shared" si="0"/>
+        <v>43167</v>
       </c>
       <c r="G23" s="20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="20"/>
@@ -3057,24 +4169,24 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
-        <v>19</v>
+      <c r="B24" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>64</v>
+        <v>56</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="F24" s="19">
         <f t="shared" si="0"/>
-        <v>43107</v>
+        <v>43168</v>
       </c>
       <c r="G24" s="20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="20"/>
@@ -3083,24 +4195,24 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>19</v>
+      <c r="B25" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="F25" s="19">
         <f t="shared" si="0"/>
-        <v>43114</v>
+        <v>43169</v>
       </c>
       <c r="G25" s="20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="20"/>
@@ -3109,24 +4221,24 @@
       </c>
     </row>
     <row r="26" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
-        <v>20</v>
+      <c r="B26" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="37" t="s">
-        <v>61</v>
+      <c r="D26" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F26" s="19">
         <f t="shared" si="0"/>
-        <v>43121</v>
+        <v>43170</v>
       </c>
       <c r="G26" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="20"/>
@@ -3135,24 +4247,24 @@
       </c>
     </row>
     <row r="27" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
-        <v>20</v>
+      <c r="B27" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="37" t="s">
-        <v>64</v>
+      <c r="D27" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F27" s="19">
         <f t="shared" si="0"/>
-        <v>43124</v>
+        <v>43172</v>
       </c>
       <c r="G27" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="20"/>
@@ -3161,24 +4273,24 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
-        <v>20</v>
+      <c r="B28" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F28" s="19">
         <f t="shared" si="0"/>
-        <v>43127</v>
+        <v>43174</v>
       </c>
       <c r="G28" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="20"/>
@@ -3188,22 +4300,23 @@
     </row>
     <row r="29" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="37" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F29" s="19">
-        <v>43146</v>
+        <f t="shared" si="0"/>
+        <v>43176</v>
       </c>
       <c r="G29" s="20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="20"/>
@@ -3213,23 +4326,23 @@
     </row>
     <row r="30" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="37" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F30" s="19">
         <f t="shared" si="0"/>
-        <v>43151</v>
+        <v>43179</v>
       </c>
       <c r="G30" s="20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="20"/>
@@ -3238,24 +4351,24 @@
       </c>
     </row>
     <row r="31" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="s">
-        <v>21</v>
+      <c r="B31" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F31" s="19">
         <f t="shared" si="0"/>
-        <v>43158</v>
+        <v>43180</v>
       </c>
       <c r="G31" s="20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="20"/>
@@ -3264,24 +4377,24 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
-        <v>22</v>
+      <c r="B32" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="37" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="F32" s="19">
         <f t="shared" si="0"/>
-        <v>43165</v>
+        <v>43181</v>
       </c>
       <c r="G32" s="20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="20"/>
@@ -3290,24 +4403,24 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="23" t="s">
-        <v>22</v>
+      <c r="B33" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="F33" s="19">
         <f t="shared" si="0"/>
-        <v>43171</v>
+        <v>43183</v>
       </c>
       <c r="G33" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="20"/>
@@ -3316,24 +4429,24 @@
       </c>
     </row>
     <row r="34" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>51</v>
+      <c r="D34" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="E34" s="36" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="F34" s="19">
         <f t="shared" si="0"/>
-        <v>43176</v>
+        <v>43185</v>
       </c>
       <c r="G34" s="20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="20"/>
@@ -3342,28 +4455,132 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>52</v>
+      <c r="B35" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="E35" s="36" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="F35" s="19">
         <f t="shared" si="0"/>
-        <v>43184</v>
+        <v>43187</v>
       </c>
       <c r="G35" s="20">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H35" s="19"/>
       <c r="I35" s="20"/>
       <c r="J35" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="19">
+        <f t="shared" si="0"/>
+        <v>43188</v>
+      </c>
+      <c r="G36" s="20">
+        <v>2</v>
+      </c>
+      <c r="H36" s="19"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="19">
+        <f t="shared" si="0"/>
+        <v>43190</v>
+      </c>
+      <c r="G37" s="20">
+        <v>2</v>
+      </c>
+      <c r="H37" s="19"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="19">
+        <f t="shared" si="0"/>
+        <v>43192</v>
+      </c>
+      <c r="G38" s="20">
+        <v>1</v>
+      </c>
+      <c r="H38" s="19"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="19">
+        <f t="shared" si="0"/>
+        <v>43193</v>
+      </c>
+      <c r="G39" s="20">
+        <v>1</v>
+      </c>
+      <c r="H39" s="19"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="22">
         <v>0</v>
       </c>
     </row>
@@ -3386,43 +4603,303 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="K6:DD35">
-    <cfRule type="expression" dxfId="41" priority="33">
+  <conditionalFormatting sqref="K6:DD36 K39:DD39">
+    <cfRule type="expression" dxfId="121" priority="113">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="35">
+    <cfRule type="expression" dxfId="120" priority="115">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="36">
+    <cfRule type="expression" dxfId="119" priority="116">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="37">
+    <cfRule type="expression" dxfId="118" priority="117">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="117" priority="118">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="39">
+    <cfRule type="expression" dxfId="116" priority="119">
       <formula>K$5=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="43">
+    <cfRule type="expression" dxfId="115" priority="123">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="114" priority="124">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36:DE36">
-    <cfRule type="expression" dxfId="33" priority="34">
+  <conditionalFormatting sqref="B40:DE40">
+    <cfRule type="expression" dxfId="113" priority="114">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:HH5">
+    <cfRule type="expression" dxfId="112" priority="120">
+      <formula>K$5=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="GQ13:HH36 DE6:HH12 GQ39:HH39">
+    <cfRule type="expression" dxfId="111" priority="81">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="82">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="83">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="84">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="85">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="86">
+      <formula>DE$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="87">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="88">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DE13:EH36 DE39:EH39">
+    <cfRule type="expression" dxfId="103" priority="105">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="106">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="107">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="108">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="109">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="110">
+      <formula>DE$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="111">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="112">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EI13:FL36 EI39:FL39">
+    <cfRule type="expression" dxfId="95" priority="97">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="98">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="99">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="100">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="101">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="102">
+      <formula>EI$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="103">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="104">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FM13:GP36 FM39:GP39">
+    <cfRule type="expression" dxfId="87" priority="89">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="90">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="91">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="92">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="93">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="94">
+      <formula>FM$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="95">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="96">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38:DD38">
+    <cfRule type="expression" dxfId="79" priority="73">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="74">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="75">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="76">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="77">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="78">
+      <formula>K$5=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="79">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="80">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="GQ38:HH38">
+    <cfRule type="expression" dxfId="71" priority="41">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="42">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="43">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="44">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="45">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="46">
+      <formula>GQ$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="47">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="48">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DE38:EH38">
+    <cfRule type="expression" dxfId="63" priority="65">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="66">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="67">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="68">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="69">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="70">
+      <formula>DE$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="71">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="72">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="EI38:FL38">
+    <cfRule type="expression" dxfId="55" priority="57">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="58">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="59">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="60">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="61">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="62">
+      <formula>EI$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="63">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="64">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FM38:GP38">
+    <cfRule type="expression" dxfId="47" priority="49">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="50">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="51">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="52">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="53">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="54">
+      <formula>FM$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="55">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="56">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K37:DD37">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>K$5=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="32" priority="40">
-      <formula>K$5=TODAY()</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="GQ13:HH35 DE6:HH12">
+  <conditionalFormatting sqref="GQ37:HH37">
     <cfRule type="expression" dxfId="31" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3439,7 +4916,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="6">
-      <formula>DE$5=period_selected</formula>
+      <formula>GQ$5=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
@@ -3448,7 +4925,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DE13:EH35">
+  <conditionalFormatting sqref="DE37:EH37">
     <cfRule type="expression" dxfId="23" priority="25">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3474,7 +4951,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="EI13:FL35">
+  <conditionalFormatting sqref="EI37:FL37">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3500,7 +4977,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FM13:GP35">
+  <conditionalFormatting sqref="FM37:GP37">
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>